<commit_message>
Fixed mistake in clue layout files
Noticed, there were two rooms labeled "O".
</commit_message>
<xml_diff>
--- a/layout/ClueLayout.xlsx
+++ b/layout/ClueLayout.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millw\CSCI 306 Workspace\ClueGame\layout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B70146F-92B8-429B-985A-50A523D1506A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="39">
   <si>
     <t>X</t>
   </si>
@@ -119,30 +138,42 @@
   </si>
   <si>
     <t>AE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F#</t>
+  </si>
+  <si>
+    <t>F*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -152,7 +183,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -192,108 +223,64 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -483,121 +470,126 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="5.43"/>
+    <col min="1" max="26" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2">
-        <f t="shared" ref="C1:S1" si="1">SUM(B1+1)</f>
+        <f t="shared" ref="C1:S1" si="0">SUM(B1+1)</f>
         <v>1</v>
       </c>
       <c r="D1" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="S1" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="T1" s="3">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2">
+        <f t="shared" ref="U1:Y1" si="1">SUM(T1+1)</f>
+        <v>19</v>
+      </c>
+      <c r="V1" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E1" s="2">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F1" s="2">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="G1" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="H1" s="2">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="I1" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="J1" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K1" s="2">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="L1" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="M1" s="2">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="N1" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="O1" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="P1" s="2">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="R1" s="2">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="S1" s="2">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="T1" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="U1" s="2">
-        <f t="shared" ref="U1:Y1" si="2">SUM(T1+1)</f>
-        <v>19</v>
-      </c>
-      <c r="V1" s="2">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="W1" s="2">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="X1" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -672,9 +664,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -749,9 +741,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -826,9 +818,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
@@ -903,9 +895,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -980,9 +972,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
@@ -1057,9 +1049,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -1134,9 +1126,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>0</v>
@@ -1211,9 +1203,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>0</v>
@@ -1288,9 +1280,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>0</v>
@@ -1365,9 +1357,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
@@ -1442,9 +1434,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>0</v>
@@ -1480,25 +1472,25 @@
         <v>1</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q13" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S13" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="S13" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>1</v>
@@ -1519,9 +1511,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -1557,25 +1549,25 @@
         <v>1</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="P14" s="23" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="R14" s="24" t="s">
-        <v>21</v>
+        <v>36</v>
+      </c>
+      <c r="R14" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="S14" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="T14" s="8" t="s">
         <v>10</v>
@@ -1596,9 +1588,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -1634,25 +1626,25 @@
         <v>1</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="P15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="R15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="S15" s="24" t="s">
-        <v>21</v>
+        <v>36</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="T15" s="5" t="s">
         <v>1</v>
@@ -1673,9 +1665,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>21</v>
@@ -1750,9 +1742,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>21</v>
@@ -1827,9 +1819,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>21</v>
@@ -1849,7 +1841,7 @@
       <c r="G18" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -1904,9 +1896,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>21</v>
@@ -1926,7 +1918,7 @@
       <c r="G19" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
@@ -1981,9 +1973,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>21</v>
@@ -2003,7 +1995,7 @@
       <c r="G20" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -2058,9 +2050,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>0</v>
@@ -2077,10 +2069,10 @@
       <c r="F21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="25" t="s">
+      <c r="G21" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I21" s="6" t="s">
@@ -2135,9 +2127,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>21</v>
@@ -2154,10 +2146,10 @@
       <c r="F22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="25" t="s">
+      <c r="G22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -2211,11 +2203,11 @@
       <c r="Y22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="Z22" s="27"/>
-    </row>
-    <row r="23">
+      <c r="Z22" s="26"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>21</v>
@@ -2232,10 +2224,10 @@
       <c r="F23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G23" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="25" t="s">
+      <c r="G23" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -2289,11 +2281,11 @@
       <c r="Y23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="Z23" s="27"/>
-    </row>
-    <row r="24">
+      <c r="Z23" s="26"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>21</v>
@@ -2310,10 +2302,10 @@
       <c r="F24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G24" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="25" t="s">
+      <c r="G24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -2367,23 +2359,23 @@
       <c r="Y24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="Z24" s="27"/>
-    </row>
-    <row r="25">
-      <c r="V25" s="27"/>
-      <c r="W25" s="27"/>
-      <c r="X25" s="27"/>
-      <c r="Y25" s="27"/>
-      <c r="Z25" s="27"/>
-    </row>
-    <row r="26">
-      <c r="V26" s="27"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="27"/>
-      <c r="Z26" s="27"/>
+      <c r="Z24" s="26"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug and made all JUnit tests pass
Code passes all tests in 306 test file and personal test file
</commit_message>
<xml_diff>
--- a/layout/ClueLayout.xlsx
+++ b/layout/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millw\CSCI 306 Workspace\ClueGame\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B70146F-92B8-429B-985A-50A523D1506A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584D53C-90BE-4487-8DB5-77EB8DD19339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="37">
   <si>
     <t>X</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>G#</t>
-  </si>
-  <si>
-    <t>W^</t>
-  </si>
-  <si>
-    <t>Wv</t>
   </si>
   <si>
     <t>H^</t>
@@ -483,7 +477,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1056,11 +1050,11 @@
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>15</v>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
@@ -1078,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>1</v>
@@ -1099,7 +1093,7 @@
         <v>12</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R8" s="6" t="s">
         <v>12</v>
@@ -1134,13 +1128,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>0</v>
@@ -1211,13 +1205,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>0</v>
@@ -1288,13 +1282,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>0</v>
@@ -1377,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>0</v>
@@ -1472,25 +1466,25 @@
         <v>1</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q13" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S13" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>1</v>
@@ -1549,25 +1543,25 @@
         <v>1</v>
       </c>
       <c r="M14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="N14" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="P14" s="23" t="s">
-        <v>38</v>
-      </c>
       <c r="Q14" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S14" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="T14" s="8" t="s">
         <v>10</v>
@@ -1626,25 +1620,25 @@
         <v>1</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S15" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="T15" s="5" t="s">
         <v>1</v>
@@ -1670,16 +1664,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>0</v>
@@ -1703,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>1</v>
@@ -1715,10 +1709,10 @@
         <v>1</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S16" s="7" t="s">
         <v>1</v>
@@ -1747,19 +1741,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>10</v>
@@ -1786,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>1</v>
@@ -1824,19 +1818,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>10</v>
@@ -1851,10 +1845,10 @@
         <v>1</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>1</v>
@@ -1863,19 +1857,19 @@
         <v>1</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P18" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R18" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="T18" s="14" t="s">
         <v>0</v>
@@ -1901,58 +1895,58 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" s="15" t="s">
+      <c r="P19" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="P19" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="Q19" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R19" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S19" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="T19" s="14" t="s">
         <v>0</v>
@@ -1978,19 +1972,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>1</v>
@@ -2005,31 +1999,31 @@
         <v>1</v>
       </c>
       <c r="K20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="R20" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S20" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="T20" s="14" t="s">
         <v>0</v>
@@ -2044,10 +2038,10 @@
         <v>0</v>
       </c>
       <c r="X20" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Y20" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -2058,16 +2052,16 @@
         <v>0</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>1</v>
@@ -2076,16 +2070,16 @@
         <v>1</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>1</v>
@@ -2094,19 +2088,19 @@
         <v>1</v>
       </c>
       <c r="O21" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P21" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="T21" s="14" t="s">
         <v>0</v>
@@ -2115,16 +2109,16 @@
         <v>0</v>
       </c>
       <c r="V21" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y21" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -2132,13 +2126,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>1</v>
@@ -2153,16 +2147,16 @@
         <v>1</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>1</v>
@@ -2171,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q22" s="14" t="s">
         <v>0</v>
@@ -2192,16 +2186,16 @@
         <v>0</v>
       </c>
       <c r="V22" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W22" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X22" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y22" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z22" s="26"/>
     </row>
@@ -2210,13 +2204,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>1</v>
@@ -2231,16 +2225,16 @@
         <v>1</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>1</v>
@@ -2249,10 +2243,10 @@
         <v>1</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q23" s="8" t="s">
         <v>10</v>
@@ -2270,16 +2264,16 @@
         <v>3</v>
       </c>
       <c r="V23" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W23" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X23" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y23" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z23" s="26"/>
     </row>
@@ -2288,13 +2282,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>1</v>
@@ -2309,16 +2303,16 @@
         <v>1</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>1</v>
@@ -2327,10 +2321,10 @@
         <v>1</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q24" s="8" t="s">
         <v>10</v>
@@ -2348,16 +2342,16 @@
         <v>3</v>
       </c>
       <c r="V24" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W24" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X24" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y24" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z24" s="26"/>
     </row>

</xml_diff>